<commit_message>
member list updated 1
</commit_message>
<xml_diff>
--- a/backend/Member Information Form For SQAC Website (Responses).xlsx
+++ b/backend/Member Information Form For SQAC Website (Responses).xlsx
@@ -1,17 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\Web dev\Side Projects\SQAC Website\sqac-website\backend\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7640"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Form Responses 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Form Responses 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="306" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="225">
   <si>
     <t>Timestamp</t>
   </si>
@@ -151,9 +159,6 @@
     <t>Jay Jariwala</t>
   </si>
   <si>
-    <t>Both</t>
-  </si>
-  <si>
     <t>https://www.instagram.com/thisisjjaay?igsh=NXlnYWdnZW5xMmxr&amp;utm_source=qr</t>
   </si>
   <si>
@@ -166,9 +171,6 @@
     <t>https://drive.google.com/open?id=1OzakOoecwLeF4JQvcCMpiDi7eleARYH3</t>
   </si>
   <si>
-    <t>App Dev and Sponsorship</t>
-  </si>
-  <si>
     <t>javintrivedi007@gmail.com</t>
   </si>
   <si>
@@ -337,9 +339,6 @@
     <t>https://drive.google.com/open?id=12nfIxrzH5BrRCjTG2jSxLCu-Yv4S6zfE</t>
   </si>
   <si>
-    <t>Web Dev and Events</t>
-  </si>
-  <si>
     <t>paavan.parmar19@gmail.com</t>
   </si>
   <si>
@@ -689,49 +688,61 @@
   </si>
   <si>
     <t>https://drive.google.com/open?id=17oj-mauavZ7lYTTV_MvHFxwA8RIIKKm7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Web Dev </t>
+  </si>
+  <si>
+    <t>App dev</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="m/d/yyyy h:mm:ss"/>
+    <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm:ss"/>
   </numFmts>
   <fonts count="7">
     <font>
-      <sz val="10.0"/>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
       <scheme val="minor"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
     </font>
     <font>
       <u/>
+      <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Roboto"/>
     </font>
@@ -741,11 +752,17 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="12">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left style="thin">
         <color rgb="FF442F65"/>
@@ -759,6 +776,7 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -773,6 +791,7 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -787,6 +806,7 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -801,6 +821,7 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -815,6 +836,7 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -829,6 +851,7 @@
       <bottom style="thin">
         <color rgb="FFFFFFFF"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -843,6 +866,7 @@
       <bottom style="thin">
         <color rgb="FFF8F9FA"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -857,6 +881,7 @@
       <bottom style="thin">
         <color rgb="FFF8F9FA"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -871,6 +896,7 @@
       <bottom style="thin">
         <color rgb="FFF8F9FA"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -885,6 +911,7 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
     <border>
       <left style="thin">
@@ -899,158 +926,148 @@
       <bottom style="thin">
         <color rgb="FF442F65"/>
       </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="23">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="2" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="4" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="5" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="8" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="9" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="10" fillId="0" fontId="1" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf borderId="11" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
-    </xf>
-    <xf borderId="11" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="center" wrapText="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="3">
     <dxf>
-      <font/>
       <fill>
-        <patternFill patternType="none"/>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFF8F9FA"/>
+          <bgColor rgb="FFF8F9FA"/>
+        </patternFill>
       </fill>
-      <border/>
     </dxf>
     <dxf>
-      <font/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFFFFF"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor rgb="FF5B3F86"/>
           <bgColor rgb="FF5B3F86"/>
         </patternFill>
       </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFFFFF"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <border/>
-    </dxf>
-    <dxf>
-      <font/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFF8F9FA"/>
-          <bgColor rgb="FFF8F9FA"/>
-        </patternFill>
-      </fill>
-      <border/>
     </dxf>
   </dxfs>
   <tableStyles count="1">
-    <tableStyle count="3" pivot="0" name="Form Responses 1-style">
-      <tableStyleElement dxfId="1" type="headerRow"/>
-      <tableStyleElement dxfId="2" type="firstRowStripe"/>
-      <tableStyleElement dxfId="3" type="secondRowStripe"/>
+    <tableStyle name="Form Responses 1-style" pivot="0" count="3">
+      <tableStyleElement type="headerRow" dxfId="2"/>
+      <tableStyleElement type="firstRowStripe" dxfId="1"/>
+      <tableStyleElement type="secondRowStripe" dxfId="0"/>
     </tableStyle>
   </tableStyles>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer"/>
-</file>
-
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" ref="A1:J34" displayName="Form_Responses" name="Form_Responses" id="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Form_Responses" displayName="Form_Responses" ref="A1:J35">
   <tableColumns count="10">
-    <tableColumn name="Timestamp" id="1"/>
-    <tableColumn name="Email Address" id="2"/>
-    <tableColumn name="Name" id="3"/>
-    <tableColumn name="Your Core Domain" id="4"/>
-    <tableColumn name="Position in SQAC" id="5"/>
-    <tableColumn name="Instagram Profile Link" id="6"/>
-    <tableColumn name="LinkedIn Profile Link" id="7"/>
-    <tableColumn name="GitHub Profile Link" id="8"/>
-    <tableColumn name="Your Image For Website " id="9"/>
-    <tableColumn name="Sub Domain" id="10"/>
+    <tableColumn id="1" name="Timestamp"/>
+    <tableColumn id="2" name="Email Address"/>
+    <tableColumn id="3" name="Name"/>
+    <tableColumn id="4" name="Your Core Domain"/>
+    <tableColumn id="5" name="Position in SQAC"/>
+    <tableColumn id="6" name="Instagram Profile Link"/>
+    <tableColumn id="7" name="LinkedIn Profile Link"/>
+    <tableColumn id="8" name="GitHub Profile Link"/>
+    <tableColumn id="9" name="Your Image For Website "/>
+    <tableColumn id="10" name="Sub Domain"/>
   </tableColumns>
-  <tableStyleInfo name="Form Responses 1-style" showColumnStripes="0" showFirstColumn="1" showLastColumn="1" showRowStripes="1"/>
+  <tableStyleInfo name="Form Responses 1-style" showFirstColumn="1" showLastColumn="1" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheets">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Sheets">
   <a:themeElements>
     <a:clrScheme name="Sheets">
       <a:dk1>
@@ -1240,31 +1257,34 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
+  <dimension ref="A1:J34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1.0" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection activeCell="B3" sqref="B3" pane="bottomLeft"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
+  <sheetFormatPr defaultColWidth="12.6328125" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col customWidth="1" min="1" max="5" width="18.88"/>
-    <col customWidth="1" min="6" max="6" width="21.25"/>
-    <col customWidth="1" min="7" max="7" width="20.0"/>
-    <col customWidth="1" min="8" max="8" width="18.88"/>
-    <col customWidth="1" min="9" max="10" width="23.0"/>
-    <col customWidth="1" min="11" max="16" width="18.88"/>
+    <col min="1" max="5" width="18.90625" customWidth="1"/>
+    <col min="6" max="6" width="21.26953125" customWidth="1"/>
+    <col min="7" max="7" width="20" customWidth="1"/>
+    <col min="8" max="8" width="18.90625" customWidth="1"/>
+    <col min="9" max="10" width="23" customWidth="1"/>
+    <col min="11" max="16" width="18.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:10" ht="15.75" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1296,7 +1316,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:10" ht="15.75" customHeight="1">
       <c r="A2" s="4">
         <v>45848.543422627314</v>
       </c>
@@ -1328,9 +1348,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="3">
+    <row r="3" spans="1:10" ht="15.75" customHeight="1">
       <c r="A3" s="8">
-        <v>45848.54517748843</v>
+        <v>45848.545177488428</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>19</v>
@@ -1360,9 +1380,9 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:10" ht="15.75" customHeight="1">
       <c r="A4" s="12">
-        <v>45848.55593174769</v>
+        <v>45848.555931747687</v>
       </c>
       <c r="B4" s="13" t="s">
         <v>27</v>
@@ -1392,9 +1412,9 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:10" ht="15.75" customHeight="1">
       <c r="A5" s="16">
-        <v>45848.55733952546</v>
+        <v>45848.557339525461</v>
       </c>
       <c r="B5" s="17" t="s">
         <v>36</v>
@@ -1424,9 +1444,9 @@
         <v>43</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:10" ht="15.75" customHeight="1">
       <c r="A6" s="12">
-        <v>45848.56112861111</v>
+        <v>45848.561128611109</v>
       </c>
       <c r="B6" s="13" t="s">
         <v>44</v>
@@ -1435,36 +1455,36 @@
         <v>45</v>
       </c>
       <c r="D6" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="14" t="s">
+      <c r="G6" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="J6" s="15" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A7" s="16">
+        <v>45848.566814918981</v>
+      </c>
+      <c r="B7" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="J6" s="15" t="s">
+      <c r="C7" s="17" t="s">
         <v>51</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" s="16">
-        <v>45848.56681491898</v>
-      </c>
-      <c r="B7" s="17" t="s">
-        <v>52</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>53</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>12</v>
@@ -1473,30 +1493,30 @@
         <v>13</v>
       </c>
       <c r="F7" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="G7" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="H7" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="I7" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="J7" s="19" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="18" t="s">
+    </row>
+    <row r="8" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A8" s="12">
+        <v>45848.569398784719</v>
+      </c>
+      <c r="B8" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="J7" s="19" t="s">
+      <c r="C8" s="13" t="s">
         <v>58</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" s="12">
-        <v>45848.56939878472</v>
-      </c>
-      <c r="B8" s="13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C8" s="13" t="s">
-        <v>60</v>
       </c>
       <c r="D8" s="13" t="s">
         <v>29</v>
@@ -1505,30 +1525,30 @@
         <v>30</v>
       </c>
       <c r="F8" s="13" t="s">
+        <v>59</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>60</v>
+      </c>
+      <c r="H8" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="I8" s="14" t="s">
         <v>62</v>
-      </c>
-      <c r="H8" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="I8" s="14" t="s">
-        <v>64</v>
       </c>
       <c r="J8" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:10" ht="15.75" customHeight="1">
       <c r="A9" s="16">
         <v>45848.572819953704</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D9" s="17" t="s">
         <v>29</v>
@@ -1537,30 +1557,30 @@
         <v>30</v>
       </c>
       <c r="F9" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="H9" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="I9" s="18" t="s">
         <v>68</v>
-      </c>
-      <c r="H9" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="I9" s="18" t="s">
-        <v>70</v>
       </c>
       <c r="J9" s="19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="10">
+    <row r="10" spans="1:10" ht="15.75" customHeight="1">
       <c r="A10" s="12">
         <v>45848.5840966088</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D10" s="13" t="s">
         <v>29</v>
@@ -1569,30 +1589,30 @@
         <v>30</v>
       </c>
       <c r="F10" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="H10" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="I10" s="14" t="s">
         <v>74</v>
-      </c>
-      <c r="H10" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="I10" s="14" t="s">
-        <v>76</v>
       </c>
       <c r="J10" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:10" ht="15.75" customHeight="1">
       <c r="A11" s="16">
-        <v>45848.58558403935</v>
+        <v>45848.585584039349</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C11" s="17" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D11" s="17" t="s">
         <v>29</v>
@@ -1601,30 +1621,30 @@
         <v>21</v>
       </c>
       <c r="F11" s="18" t="s">
+        <v>77</v>
+      </c>
+      <c r="G11" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="H11" s="18" t="s">
         <v>79</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="I11" s="18" t="s">
         <v>80</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="J11" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="I11" s="18" t="s">
-        <v>82</v>
-      </c>
-      <c r="J11" s="19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12">
+    </row>
+    <row r="12" spans="1:10" ht="15.75" customHeight="1">
       <c r="A12" s="12">
         <v>45848.59035131945</v>
       </c>
       <c r="B12" s="13" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="C12" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D12" s="13" t="s">
         <v>12</v>
@@ -1633,30 +1653,30 @@
         <v>21</v>
       </c>
       <c r="F12" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="G12" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="H12" s="14" t="s">
         <v>86</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="I12" s="14" t="s">
         <v>87</v>
-      </c>
-      <c r="H12" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I12" s="14" t="s">
-        <v>89</v>
       </c>
       <c r="J12" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:10" ht="15.75" customHeight="1">
       <c r="A13" s="16">
-        <v>45848.59055353009</v>
+        <v>45848.590553530092</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="D13" s="17" t="s">
         <v>29</v>
@@ -1665,30 +1685,30 @@
         <v>30</v>
       </c>
       <c r="F13" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="H13" s="18" t="s">
         <v>92</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="I13" s="18" t="s">
         <v>93</v>
-      </c>
-      <c r="H13" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="I13" s="18" t="s">
-        <v>95</v>
       </c>
       <c r="J13" s="19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:10" ht="15.75" customHeight="1">
       <c r="A14" s="12">
-        <v>45848.59883337963</v>
+        <v>45848.598833379627</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C14" s="13" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D14" s="13" t="s">
         <v>29</v>
@@ -1697,62 +1717,62 @@
         <v>30</v>
       </c>
       <c r="F14" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="H14" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="G14" s="14" t="s">
+      <c r="I14" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="H14" s="14" t="s">
+      <c r="J14" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A15" s="16">
+        <v>45848.599338726854</v>
+      </c>
+      <c r="B15" s="17" t="s">
         <v>100</v>
       </c>
-      <c r="I14" s="14" t="s">
+      <c r="C15" s="17" t="s">
         <v>101</v>
       </c>
-      <c r="J14" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="16">
-        <v>45848.59933872685</v>
-      </c>
-      <c r="B15" s="17" t="s">
-        <v>102</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>103</v>
-      </c>
       <c r="D15" s="17" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>30</v>
       </c>
       <c r="F15" s="18" t="s">
+        <v>102</v>
+      </c>
+      <c r="G15" s="18" t="s">
+        <v>103</v>
+      </c>
+      <c r="H15" s="18" t="s">
         <v>104</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="I15" s="18" t="s">
         <v>105</v>
       </c>
-      <c r="H15" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="I15" s="18" t="s">
-        <v>107</v>
-      </c>
       <c r="J15" s="19" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="16">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" customHeight="1">
       <c r="A16" s="12">
         <v>45848.627040046296</v>
       </c>
       <c r="B16" s="13" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="C16" s="13" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="D16" s="13" t="s">
         <v>29</v>
@@ -1761,30 +1781,30 @@
         <v>13</v>
       </c>
       <c r="F16" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="G16" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="H16" s="13" t="s">
+        <v>110</v>
+      </c>
+      <c r="I16" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="G16" s="14" t="s">
+      <c r="J16" s="15" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A17" s="16">
+        <v>45848.645386655087</v>
+      </c>
+      <c r="B17" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="H16" s="13" t="s">
+      <c r="C17" s="17" t="s">
         <v>113</v>
-      </c>
-      <c r="I16" s="14" t="s">
-        <v>114</v>
-      </c>
-      <c r="J16" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="16">
-        <v>45848.64538665509</v>
-      </c>
-      <c r="B17" s="17" t="s">
-        <v>115</v>
-      </c>
-      <c r="C17" s="17" t="s">
-        <v>116</v>
       </c>
       <c r="D17" s="17" t="s">
         <v>29</v>
@@ -1793,30 +1813,30 @@
         <v>21</v>
       </c>
       <c r="F17" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>116</v>
+      </c>
+      <c r="I17" s="18" t="s">
         <v>117</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="J17" s="19" t="s">
         <v>118</v>
       </c>
-      <c r="H17" s="18" t="s">
-        <v>119</v>
-      </c>
-      <c r="I17" s="18" t="s">
-        <v>120</v>
-      </c>
-      <c r="J17" s="19" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="18">
+    </row>
+    <row r="18" spans="1:10" ht="15.75" customHeight="1">
       <c r="A18" s="12">
         <v>45848.65894390046</v>
       </c>
       <c r="B18" s="13" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C18" s="13" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="D18" s="13" t="s">
         <v>12</v>
@@ -1825,30 +1845,30 @@
         <v>38</v>
       </c>
       <c r="F18" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="G18" s="14" t="s">
+        <v>122</v>
+      </c>
+      <c r="H18" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="I18" s="14" t="s">
         <v>124</v>
       </c>
-      <c r="G18" s="14" t="s">
+      <c r="J18" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="H18" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="I18" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="J18" s="15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="19">
+    </row>
+    <row r="19" spans="1:10" ht="15.75" customHeight="1">
       <c r="A19" s="16">
         <v>45848.679524583335</v>
       </c>
       <c r="B19" s="17" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="C19" s="17" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="D19" s="17" t="s">
         <v>29</v>
@@ -1857,30 +1877,30 @@
         <v>21</v>
       </c>
       <c r="F19" s="18" t="s">
+        <v>128</v>
+      </c>
+      <c r="G19" s="18" t="s">
+        <v>129</v>
+      </c>
+      <c r="H19" s="18" t="s">
+        <v>130</v>
+      </c>
+      <c r="I19" s="18" t="s">
         <v>131</v>
-      </c>
-      <c r="G19" s="18" t="s">
-        <v>132</v>
-      </c>
-      <c r="H19" s="18" t="s">
-        <v>133</v>
-      </c>
-      <c r="I19" s="18" t="s">
-        <v>134</v>
       </c>
       <c r="J19" s="19" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="20">
+    <row r="20" spans="1:10" ht="15.75" customHeight="1">
       <c r="A20" s="12">
-        <v>45848.68835332176</v>
+        <v>45848.688353321762</v>
       </c>
       <c r="B20" s="13" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C20" s="13" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="D20" s="13" t="s">
         <v>29</v>
@@ -1889,30 +1909,30 @@
         <v>13</v>
       </c>
       <c r="F20" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="G20" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="H20" s="14" t="s">
+        <v>136</v>
+      </c>
+      <c r="I20" s="14" t="s">
         <v>137</v>
-      </c>
-      <c r="G20" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="H20" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="I20" s="14" t="s">
-        <v>140</v>
       </c>
       <c r="J20" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21">
+    <row r="21" spans="1:10" ht="15.75" customHeight="1">
       <c r="A21" s="16">
-        <v>45848.76306925926</v>
+        <v>45848.763069259257</v>
       </c>
       <c r="B21" s="17" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C21" s="17" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="D21" s="17" t="s">
         <v>12</v>
@@ -1921,30 +1941,30 @@
         <v>30</v>
       </c>
       <c r="F21" s="18" t="s">
+        <v>140</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>141</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>142</v>
+      </c>
+      <c r="I21" s="18" t="s">
         <v>143</v>
-      </c>
-      <c r="G21" s="18" t="s">
-        <v>144</v>
-      </c>
-      <c r="H21" s="18" t="s">
-        <v>145</v>
-      </c>
-      <c r="I21" s="18" t="s">
-        <v>146</v>
       </c>
       <c r="J21" s="19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:10" ht="15.75" customHeight="1">
       <c r="A22" s="12">
         <v>45849.361394328706</v>
       </c>
       <c r="B22" s="13" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C22" s="13" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="D22" s="13" t="s">
         <v>29</v>
@@ -1953,30 +1973,30 @@
         <v>21</v>
       </c>
       <c r="F22" s="14" t="s">
+        <v>146</v>
+      </c>
+      <c r="G22" s="14" t="s">
+        <v>147</v>
+      </c>
+      <c r="H22" s="14" t="s">
+        <v>148</v>
+      </c>
+      <c r="I22" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="J22" s="15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A23" s="16">
+        <v>45849.373223460643</v>
+      </c>
+      <c r="B23" s="17" t="s">
         <v>150</v>
       </c>
-      <c r="H22" s="14" t="s">
+      <c r="C23" s="17" t="s">
         <v>151</v>
-      </c>
-      <c r="I22" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="J22" s="15" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="16">
-        <v>45849.37322346064</v>
-      </c>
-      <c r="B23" s="17" t="s">
-        <v>153</v>
-      </c>
-      <c r="C23" s="17" t="s">
-        <v>154</v>
       </c>
       <c r="D23" s="17" t="s">
         <v>12</v>
@@ -1985,30 +2005,30 @@
         <v>30</v>
       </c>
       <c r="F23" s="18" t="s">
+        <v>152</v>
+      </c>
+      <c r="G23" s="18" t="s">
+        <v>153</v>
+      </c>
+      <c r="H23" s="18" t="s">
+        <v>154</v>
+      </c>
+      <c r="I23" s="18" t="s">
         <v>155</v>
       </c>
-      <c r="G23" s="18" t="s">
+      <c r="J23" s="19" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="15.75" customHeight="1">
+      <c r="A24" s="12">
+        <v>45849.448668263889</v>
+      </c>
+      <c r="B24" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="H23" s="18" t="s">
+      <c r="C24" s="13" t="s">
         <v>157</v>
-      </c>
-      <c r="I23" s="18" t="s">
-        <v>158</v>
-      </c>
-      <c r="J23" s="19" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="12">
-        <v>45849.44866826389</v>
-      </c>
-      <c r="B24" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="C24" s="13" t="s">
-        <v>160</v>
       </c>
       <c r="D24" s="13" t="s">
         <v>12</v>
@@ -2017,30 +2037,30 @@
         <v>21</v>
       </c>
       <c r="F24" s="14" t="s">
+        <v>158</v>
+      </c>
+      <c r="G24" s="14" t="s">
+        <v>159</v>
+      </c>
+      <c r="H24" s="14" t="s">
+        <v>160</v>
+      </c>
+      <c r="I24" s="14" t="s">
         <v>161</v>
       </c>
-      <c r="G24" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="H24" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="I24" s="14" t="s">
-        <v>164</v>
-      </c>
       <c r="J24" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="15.75" customHeight="1">
       <c r="A25" s="16">
         <v>45849.560061041666</v>
       </c>
       <c r="B25" s="17" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="D25" s="17" t="s">
         <v>29</v>
@@ -2049,30 +2069,30 @@
         <v>38</v>
       </c>
       <c r="F25" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="H25" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="I25" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="G25" s="18" t="s">
+      <c r="J25" s="19" t="s">
         <v>168</v>
       </c>
-      <c r="H25" s="18" t="s">
-        <v>169</v>
-      </c>
-      <c r="I25" s="18" t="s">
-        <v>170</v>
-      </c>
-      <c r="J25" s="19" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="26">
+    </row>
+    <row r="26" spans="1:10" ht="12.5">
       <c r="A26" s="12">
         <v>45849.87844818287</v>
       </c>
       <c r="B26" s="13" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="D26" s="13" t="s">
         <v>29</v>
@@ -2081,30 +2101,30 @@
         <v>30</v>
       </c>
       <c r="F26" s="14" t="s">
+        <v>171</v>
+      </c>
+      <c r="G26" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="H26" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="I26" s="14" t="s">
         <v>174</v>
       </c>
-      <c r="G26" s="14" t="s">
+      <c r="J26" s="15" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" ht="12.5">
+      <c r="A27" s="16">
+        <v>45849.906536956019</v>
+      </c>
+      <c r="B27" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="H26" s="14" t="s">
+      <c r="C27" s="17" t="s">
         <v>176</v>
-      </c>
-      <c r="I26" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="J26" s="15" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" s="16">
-        <v>45849.90653695602</v>
-      </c>
-      <c r="B27" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="C27" s="17" t="s">
-        <v>179</v>
       </c>
       <c r="D27" s="17" t="s">
         <v>12</v>
@@ -2113,30 +2133,30 @@
         <v>21</v>
       </c>
       <c r="F27" s="18" t="s">
+        <v>177</v>
+      </c>
+      <c r="G27" s="18" t="s">
+        <v>178</v>
+      </c>
+      <c r="H27" s="18" t="s">
+        <v>179</v>
+      </c>
+      <c r="I27" s="18" t="s">
         <v>180</v>
-      </c>
-      <c r="G27" s="18" t="s">
-        <v>181</v>
-      </c>
-      <c r="H27" s="18" t="s">
-        <v>182</v>
-      </c>
-      <c r="I27" s="18" t="s">
-        <v>183</v>
       </c>
       <c r="J27" s="19" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:10" ht="12.5">
       <c r="A28" s="12">
-        <v>45849.98335381944</v>
+        <v>45849.983353819443</v>
       </c>
       <c r="B28" s="13" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C28" s="13" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="D28" s="13" t="s">
         <v>29</v>
@@ -2145,30 +2165,30 @@
         <v>30</v>
       </c>
       <c r="F28" s="14" t="s">
+        <v>183</v>
+      </c>
+      <c r="G28" s="14" t="s">
+        <v>184</v>
+      </c>
+      <c r="H28" s="14" t="s">
+        <v>185</v>
+      </c>
+      <c r="I28" s="14" t="s">
         <v>186</v>
       </c>
-      <c r="G28" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="H28" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="I28" s="14" t="s">
-        <v>189</v>
-      </c>
       <c r="J28" s="15" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="29">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" ht="12.5">
       <c r="A29" s="16">
         <v>45850.044633854166</v>
       </c>
       <c r="B29" s="17" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C29" s="17" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="D29" s="17" t="s">
         <v>12</v>
@@ -2177,30 +2197,30 @@
         <v>30</v>
       </c>
       <c r="F29" s="18" t="s">
+        <v>189</v>
+      </c>
+      <c r="G29" s="18" t="s">
+        <v>190</v>
+      </c>
+      <c r="H29" s="18" t="s">
+        <v>191</v>
+      </c>
+      <c r="I29" s="18" t="s">
         <v>192</v>
-      </c>
-      <c r="G29" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="H29" s="18" t="s">
-        <v>194</v>
-      </c>
-      <c r="I29" s="18" t="s">
-        <v>195</v>
       </c>
       <c r="J29" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:10" ht="12.5">
       <c r="A30" s="12">
-        <v>45850.90540725694</v>
+        <v>45850.905407256942</v>
       </c>
       <c r="B30" s="13" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C30" s="13" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="D30" s="13" t="s">
         <v>29</v>
@@ -2209,30 +2229,30 @@
         <v>21</v>
       </c>
       <c r="F30" s="14" t="s">
+        <v>195</v>
+      </c>
+      <c r="G30" s="14" t="s">
+        <v>196</v>
+      </c>
+      <c r="H30" s="14" t="s">
+        <v>197</v>
+      </c>
+      <c r="I30" s="14" t="s">
         <v>198</v>
-      </c>
-      <c r="G30" s="14" t="s">
-        <v>199</v>
-      </c>
-      <c r="H30" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="I30" s="14" t="s">
-        <v>201</v>
       </c>
       <c r="J30" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:10" ht="12.5">
       <c r="A31" s="16">
-        <v>45850.92842804398</v>
+        <v>45850.928428043982</v>
       </c>
       <c r="B31" s="17" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C31" s="17" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="D31" s="17" t="s">
         <v>12</v>
@@ -2241,62 +2261,62 @@
         <v>30</v>
       </c>
       <c r="F31" s="18" t="s">
+        <v>201</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>202</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>203</v>
+      </c>
+      <c r="I31" s="18" t="s">
         <v>204</v>
-      </c>
-      <c r="G31" s="18" t="s">
-        <v>205</v>
-      </c>
-      <c r="H31" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="I31" s="18" t="s">
-        <v>207</v>
       </c>
       <c r="J31" s="19" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:10" ht="12.5">
       <c r="A32" s="12">
-        <v>45850.94799134259</v>
+        <v>45850.947991342589</v>
       </c>
       <c r="B32" s="13" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C32" s="13" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="D32" s="13" t="s">
         <v>29</v>
       </c>
       <c r="E32" s="13" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="F32" s="14" t="s">
+        <v>207</v>
+      </c>
+      <c r="G32" s="14" t="s">
+        <v>208</v>
+      </c>
+      <c r="H32" s="14" t="s">
+        <v>209</v>
+      </c>
+      <c r="I32" s="14" t="s">
         <v>210</v>
-      </c>
-      <c r="G32" s="14" t="s">
-        <v>211</v>
-      </c>
-      <c r="H32" s="14" t="s">
-        <v>212</v>
-      </c>
-      <c r="I32" s="14" t="s">
-        <v>213</v>
       </c>
       <c r="J32" s="15" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:10" ht="12.5">
       <c r="A33" s="16">
-        <v>45852.70317234954</v>
+        <v>45852.703172349538</v>
       </c>
       <c r="B33" s="17" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="D33" s="17" t="s">
         <v>29</v>
@@ -2305,185 +2325,188 @@
         <v>30</v>
       </c>
       <c r="F33" s="18" t="s">
+        <v>213</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>214</v>
+      </c>
+      <c r="H33" s="17" t="s">
+        <v>215</v>
+      </c>
+      <c r="I33" s="18" t="s">
         <v>216</v>
       </c>
-      <c r="G33" s="18" t="s">
-        <v>217</v>
-      </c>
-      <c r="H33" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="I33" s="18" t="s">
-        <v>219</v>
-      </c>
       <c r="J33" s="19" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="34">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" ht="12.5">
       <c r="A34" s="20">
         <v>45866.404996261575</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C34" s="21" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>46</v>
+        <v>29</v>
       </c>
       <c r="E34" s="21" t="s">
         <v>38</v>
       </c>
       <c r="F34" s="22" t="s">
+        <v>219</v>
+      </c>
+      <c r="G34" s="22" t="s">
+        <v>220</v>
+      </c>
+      <c r="H34" s="22" t="s">
+        <v>221</v>
+      </c>
+      <c r="I34" s="22" t="s">
         <v>222</v>
       </c>
-      <c r="G34" s="22" t="s">
-        <v>223</v>
-      </c>
-      <c r="H34" s="22" t="s">
-        <v>224</v>
-      </c>
-      <c r="I34" s="22" t="s">
-        <v>225</v>
+      <c r="J34" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink r:id="rId1" ref="F2"/>
-    <hyperlink r:id="rId2" ref="G2"/>
-    <hyperlink r:id="rId3" ref="H2"/>
-    <hyperlink r:id="rId4" ref="I2"/>
-    <hyperlink r:id="rId5" ref="F3"/>
-    <hyperlink r:id="rId6" ref="G3"/>
-    <hyperlink r:id="rId7" ref="H3"/>
-    <hyperlink r:id="rId8" ref="I3"/>
-    <hyperlink r:id="rId9" ref="F4"/>
-    <hyperlink r:id="rId10" ref="G4"/>
-    <hyperlink r:id="rId11" ref="H4"/>
-    <hyperlink r:id="rId12" ref="I4"/>
-    <hyperlink r:id="rId13" ref="F5"/>
-    <hyperlink r:id="rId14" ref="G5"/>
-    <hyperlink r:id="rId15" ref="H5"/>
-    <hyperlink r:id="rId16" ref="I5"/>
-    <hyperlink r:id="rId17" ref="F6"/>
-    <hyperlink r:id="rId18" ref="G6"/>
-    <hyperlink r:id="rId19" ref="H6"/>
-    <hyperlink r:id="rId20" ref="I6"/>
-    <hyperlink r:id="rId21" ref="F7"/>
-    <hyperlink r:id="rId22" ref="G7"/>
-    <hyperlink r:id="rId23" ref="H7"/>
-    <hyperlink r:id="rId24" ref="I7"/>
-    <hyperlink r:id="rId25" ref="G8"/>
-    <hyperlink r:id="rId26" ref="H8"/>
-    <hyperlink r:id="rId27" ref="I8"/>
-    <hyperlink r:id="rId28" ref="F9"/>
-    <hyperlink r:id="rId29" ref="G9"/>
-    <hyperlink r:id="rId30" ref="H9"/>
-    <hyperlink r:id="rId31" ref="I9"/>
-    <hyperlink r:id="rId32" ref="F10"/>
-    <hyperlink r:id="rId33" ref="G10"/>
-    <hyperlink r:id="rId34" ref="H10"/>
-    <hyperlink r:id="rId35" ref="I10"/>
-    <hyperlink r:id="rId36" ref="F11"/>
-    <hyperlink r:id="rId37" ref="G11"/>
-    <hyperlink r:id="rId38" ref="H11"/>
-    <hyperlink r:id="rId39" ref="I11"/>
-    <hyperlink r:id="rId40" ref="F12"/>
-    <hyperlink r:id="rId41" ref="G12"/>
-    <hyperlink r:id="rId42" ref="H12"/>
-    <hyperlink r:id="rId43" ref="I12"/>
-    <hyperlink r:id="rId44" ref="F13"/>
-    <hyperlink r:id="rId45" ref="G13"/>
-    <hyperlink r:id="rId46" ref="H13"/>
-    <hyperlink r:id="rId47" ref="I13"/>
-    <hyperlink r:id="rId48" ref="F14"/>
-    <hyperlink r:id="rId49" ref="G14"/>
-    <hyperlink r:id="rId50" ref="H14"/>
-    <hyperlink r:id="rId51" ref="I14"/>
-    <hyperlink r:id="rId52" ref="F15"/>
-    <hyperlink r:id="rId53" ref="G15"/>
-    <hyperlink r:id="rId54" ref="H15"/>
-    <hyperlink r:id="rId55" ref="I15"/>
-    <hyperlink r:id="rId56" ref="F16"/>
-    <hyperlink r:id="rId57" ref="G16"/>
-    <hyperlink r:id="rId58" ref="I16"/>
-    <hyperlink r:id="rId59" ref="F17"/>
-    <hyperlink r:id="rId60" ref="G17"/>
-    <hyperlink r:id="rId61" ref="H17"/>
-    <hyperlink r:id="rId62" ref="I17"/>
-    <hyperlink r:id="rId63" ref="F18"/>
-    <hyperlink r:id="rId64" ref="G18"/>
-    <hyperlink r:id="rId65" ref="H18"/>
-    <hyperlink r:id="rId66" ref="I18"/>
-    <hyperlink r:id="rId67" ref="F19"/>
-    <hyperlink r:id="rId68" ref="G19"/>
-    <hyperlink r:id="rId69" ref="H19"/>
-    <hyperlink r:id="rId70" ref="I19"/>
-    <hyperlink r:id="rId71" ref="F20"/>
-    <hyperlink r:id="rId72" ref="G20"/>
-    <hyperlink r:id="rId73" ref="H20"/>
-    <hyperlink r:id="rId74" ref="I20"/>
-    <hyperlink r:id="rId75" ref="F21"/>
-    <hyperlink r:id="rId76" ref="G21"/>
-    <hyperlink r:id="rId77" ref="H21"/>
-    <hyperlink r:id="rId78" ref="I21"/>
-    <hyperlink r:id="rId79" ref="F22"/>
-    <hyperlink r:id="rId80" ref="G22"/>
-    <hyperlink r:id="rId81" ref="H22"/>
-    <hyperlink r:id="rId82" ref="I22"/>
-    <hyperlink r:id="rId83" ref="F23"/>
-    <hyperlink r:id="rId84" ref="G23"/>
-    <hyperlink r:id="rId85" ref="H23"/>
-    <hyperlink r:id="rId86" ref="I23"/>
-    <hyperlink r:id="rId87" ref="F24"/>
-    <hyperlink r:id="rId88" ref="G24"/>
-    <hyperlink r:id="rId89" ref="H24"/>
-    <hyperlink r:id="rId90" ref="I24"/>
-    <hyperlink r:id="rId91" ref="F25"/>
-    <hyperlink r:id="rId92" ref="G25"/>
-    <hyperlink r:id="rId93" ref="H25"/>
-    <hyperlink r:id="rId94" ref="I25"/>
-    <hyperlink r:id="rId95" ref="F26"/>
-    <hyperlink r:id="rId96" ref="G26"/>
-    <hyperlink r:id="rId97" ref="H26"/>
-    <hyperlink r:id="rId98" ref="I26"/>
-    <hyperlink r:id="rId99" ref="F27"/>
-    <hyperlink r:id="rId100" ref="G27"/>
-    <hyperlink r:id="rId101" ref="H27"/>
-    <hyperlink r:id="rId102" ref="I27"/>
-    <hyperlink r:id="rId103" ref="F28"/>
-    <hyperlink r:id="rId104" ref="G28"/>
-    <hyperlink r:id="rId105" ref="H28"/>
-    <hyperlink r:id="rId106" ref="I28"/>
-    <hyperlink r:id="rId107" ref="F29"/>
-    <hyperlink r:id="rId108" ref="G29"/>
-    <hyperlink r:id="rId109" ref="H29"/>
-    <hyperlink r:id="rId110" ref="I29"/>
-    <hyperlink r:id="rId111" ref="F30"/>
-    <hyperlink r:id="rId112" ref="G30"/>
-    <hyperlink r:id="rId113" ref="H30"/>
-    <hyperlink r:id="rId114" ref="I30"/>
-    <hyperlink r:id="rId115" ref="F31"/>
-    <hyperlink r:id="rId116" ref="G31"/>
-    <hyperlink r:id="rId117" ref="H31"/>
-    <hyperlink r:id="rId118" ref="I31"/>
-    <hyperlink r:id="rId119" ref="F32"/>
-    <hyperlink r:id="rId120" ref="G32"/>
-    <hyperlink r:id="rId121" ref="H32"/>
-    <hyperlink r:id="rId122" ref="I32"/>
-    <hyperlink r:id="rId123" ref="F33"/>
-    <hyperlink r:id="rId124" ref="G33"/>
-    <hyperlink r:id="rId125" ref="I33"/>
-    <hyperlink r:id="rId126" ref="F34"/>
-    <hyperlink r:id="rId127" ref="G34"/>
-    <hyperlink r:id="rId128" ref="H34"/>
-    <hyperlink r:id="rId129" ref="I34"/>
+    <hyperlink ref="F2" r:id="rId1"/>
+    <hyperlink ref="G2" r:id="rId2"/>
+    <hyperlink ref="H2" r:id="rId3"/>
+    <hyperlink ref="I2" r:id="rId4"/>
+    <hyperlink ref="F3" r:id="rId5"/>
+    <hyperlink ref="G3" r:id="rId6"/>
+    <hyperlink ref="H3" r:id="rId7"/>
+    <hyperlink ref="I3" r:id="rId8"/>
+    <hyperlink ref="F4" r:id="rId9"/>
+    <hyperlink ref="G4" r:id="rId10"/>
+    <hyperlink ref="H4" r:id="rId11"/>
+    <hyperlink ref="I4" r:id="rId12"/>
+    <hyperlink ref="F5" r:id="rId13"/>
+    <hyperlink ref="G5" r:id="rId14"/>
+    <hyperlink ref="H5" r:id="rId15"/>
+    <hyperlink ref="I5" r:id="rId16"/>
+    <hyperlink ref="F6" r:id="rId17"/>
+    <hyperlink ref="G6" r:id="rId18"/>
+    <hyperlink ref="H6" r:id="rId19"/>
+    <hyperlink ref="I6" r:id="rId20"/>
+    <hyperlink ref="F7" r:id="rId21"/>
+    <hyperlink ref="G7" r:id="rId22"/>
+    <hyperlink ref="H7" r:id="rId23"/>
+    <hyperlink ref="I7" r:id="rId24"/>
+    <hyperlink ref="G8" r:id="rId25"/>
+    <hyperlink ref="H8" r:id="rId26"/>
+    <hyperlink ref="I8" r:id="rId27"/>
+    <hyperlink ref="F9" r:id="rId28"/>
+    <hyperlink ref="G9" r:id="rId29"/>
+    <hyperlink ref="H9" r:id="rId30"/>
+    <hyperlink ref="I9" r:id="rId31"/>
+    <hyperlink ref="F10" r:id="rId32"/>
+    <hyperlink ref="G10" r:id="rId33"/>
+    <hyperlink ref="H10" r:id="rId34"/>
+    <hyperlink ref="I10" r:id="rId35"/>
+    <hyperlink ref="F11" r:id="rId36"/>
+    <hyperlink ref="G11" r:id="rId37"/>
+    <hyperlink ref="H11" r:id="rId38"/>
+    <hyperlink ref="I11" r:id="rId39"/>
+    <hyperlink ref="F12" r:id="rId40"/>
+    <hyperlink ref="G12" r:id="rId41"/>
+    <hyperlink ref="H12" r:id="rId42"/>
+    <hyperlink ref="I12" r:id="rId43"/>
+    <hyperlink ref="F13" r:id="rId44"/>
+    <hyperlink ref="G13" r:id="rId45"/>
+    <hyperlink ref="H13" r:id="rId46"/>
+    <hyperlink ref="I13" r:id="rId47"/>
+    <hyperlink ref="F14" r:id="rId48"/>
+    <hyperlink ref="G14" r:id="rId49"/>
+    <hyperlink ref="H14" r:id="rId50"/>
+    <hyperlink ref="I14" r:id="rId51"/>
+    <hyperlink ref="F15" r:id="rId52"/>
+    <hyperlink ref="G15" r:id="rId53"/>
+    <hyperlink ref="H15" r:id="rId54"/>
+    <hyperlink ref="I15" r:id="rId55"/>
+    <hyperlink ref="F16" r:id="rId56"/>
+    <hyperlink ref="G16" r:id="rId57"/>
+    <hyperlink ref="I16" r:id="rId58"/>
+    <hyperlink ref="F17" r:id="rId59"/>
+    <hyperlink ref="G17" r:id="rId60"/>
+    <hyperlink ref="H17" r:id="rId61"/>
+    <hyperlink ref="I17" r:id="rId62"/>
+    <hyperlink ref="F18" r:id="rId63"/>
+    <hyperlink ref="G18" r:id="rId64"/>
+    <hyperlink ref="H18" r:id="rId65"/>
+    <hyperlink ref="I18" r:id="rId66"/>
+    <hyperlink ref="F19" r:id="rId67"/>
+    <hyperlink ref="G19" r:id="rId68"/>
+    <hyperlink ref="H19" r:id="rId69"/>
+    <hyperlink ref="I19" r:id="rId70"/>
+    <hyperlink ref="F20" r:id="rId71"/>
+    <hyperlink ref="G20" r:id="rId72"/>
+    <hyperlink ref="H20" r:id="rId73"/>
+    <hyperlink ref="I20" r:id="rId74"/>
+    <hyperlink ref="F21" r:id="rId75"/>
+    <hyperlink ref="G21" r:id="rId76"/>
+    <hyperlink ref="H21" r:id="rId77"/>
+    <hyperlink ref="I21" r:id="rId78"/>
+    <hyperlink ref="F22" r:id="rId79"/>
+    <hyperlink ref="G22" r:id="rId80"/>
+    <hyperlink ref="H22" r:id="rId81"/>
+    <hyperlink ref="I22" r:id="rId82"/>
+    <hyperlink ref="F23" r:id="rId83"/>
+    <hyperlink ref="G23" r:id="rId84"/>
+    <hyperlink ref="H23" r:id="rId85"/>
+    <hyperlink ref="I23" r:id="rId86"/>
+    <hyperlink ref="F24" r:id="rId87"/>
+    <hyperlink ref="G24" r:id="rId88"/>
+    <hyperlink ref="H24" r:id="rId89"/>
+    <hyperlink ref="I24" r:id="rId90"/>
+    <hyperlink ref="F25" r:id="rId91"/>
+    <hyperlink ref="G25" r:id="rId92"/>
+    <hyperlink ref="H25" r:id="rId93"/>
+    <hyperlink ref="I25" r:id="rId94"/>
+    <hyperlink ref="F26" r:id="rId95"/>
+    <hyperlink ref="G26" r:id="rId96"/>
+    <hyperlink ref="H26" r:id="rId97"/>
+    <hyperlink ref="I26" r:id="rId98"/>
+    <hyperlink ref="F27" r:id="rId99"/>
+    <hyperlink ref="G27" r:id="rId100"/>
+    <hyperlink ref="H27" r:id="rId101"/>
+    <hyperlink ref="I27" r:id="rId102"/>
+    <hyperlink ref="F28" r:id="rId103"/>
+    <hyperlink ref="G28" r:id="rId104"/>
+    <hyperlink ref="H28" r:id="rId105"/>
+    <hyperlink ref="I28" r:id="rId106"/>
+    <hyperlink ref="F29" r:id="rId107"/>
+    <hyperlink ref="G29" r:id="rId108"/>
+    <hyperlink ref="H29" r:id="rId109"/>
+    <hyperlink ref="I29" r:id="rId110"/>
+    <hyperlink ref="F30" r:id="rId111"/>
+    <hyperlink ref="G30" r:id="rId112"/>
+    <hyperlink ref="H30" r:id="rId113"/>
+    <hyperlink ref="I30" r:id="rId114"/>
+    <hyperlink ref="F31" r:id="rId115"/>
+    <hyperlink ref="G31" r:id="rId116"/>
+    <hyperlink ref="H31" r:id="rId117"/>
+    <hyperlink ref="I31" r:id="rId118"/>
+    <hyperlink ref="F32" r:id="rId119"/>
+    <hyperlink ref="G32" r:id="rId120"/>
+    <hyperlink ref="H32" r:id="rId121"/>
+    <hyperlink ref="I32" r:id="rId122"/>
+    <hyperlink ref="F33" r:id="rId123"/>
+    <hyperlink ref="G33" r:id="rId124"/>
+    <hyperlink ref="I33" r:id="rId125"/>
+    <hyperlink ref="F34" r:id="rId126"/>
+    <hyperlink ref="G34" r:id="rId127"/>
+    <hyperlink ref="H34" r:id="rId128"/>
+    <hyperlink ref="I34" r:id="rId129"/>
   </hyperlinks>
-  <drawing r:id="rId130"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId132"/>
+    <tablePart r:id="rId130"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix: Updated member list
</commit_message>
<xml_diff>
--- a/backend/Member Information Form For SQAC Website (Responses).xlsx
+++ b/backend/Member Information Form For SQAC Website (Responses).xlsx
@@ -76,178 +76,178 @@
     <t>Simran Nayak</t>
   </si>
   <si>
+    <t>https://www.instagram.com/justanother.simrann?igsh=MWVncndtM2swNnJ4dw%3D%3D&amp;utm_source=qr</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/simran-nayak-865692297?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=ios_app</t>
+  </si>
+  <si>
+    <t>https://github.com/simrann130904?tab=repositories</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1SXRdcVF9FQYYoQldNtodKB_xiCPzaOHE</t>
+  </si>
+  <si>
+    <t>PR</t>
+  </si>
+  <si>
+    <t>christin.kjoseph@gmail.com</t>
+  </si>
+  <si>
+    <t>Christin Kurian Joseph</t>
+  </si>
+  <si>
+    <t>Technical</t>
+  </si>
+  <si>
+    <t>Member</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/christin._.kj?igsh=MWwwcG02ZTl6YXlyNg==</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/christin-joseph-a12a39252?</t>
+  </si>
+  <si>
+    <t>https://github.com/ChristinJoseph</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1mgAX4od3RahXehy42KVxSZ3eA5pFRv6s</t>
+  </si>
+  <si>
+    <t>Web Dev</t>
+  </si>
+  <si>
+    <t>priyanshuvasudev2005@gmail.com</t>
+  </si>
+  <si>
+    <t>Priyanshu Vasudev</t>
+  </si>
+  <si>
+    <t>Board Member</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/priyanshu.vasudev/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/priyanshu-vasudev-off/</t>
+  </si>
+  <si>
+    <t>https://github.com/Priyanshu2608</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1ZxcPvrcPgjfsAxP7CrYr6JdEiQIhWm_8</t>
+  </si>
+  <si>
+    <t>Technical Lead</t>
+  </si>
+  <si>
+    <t>jjariwala111@gmail.com</t>
+  </si>
+  <si>
+    <t>Jay Jariwala</t>
+  </si>
+  <si>
+    <t>Both</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/thisisjjaay?igsh=NXlnYWdnZW5xMmxr&amp;utm_source=qr</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/jay-jariwala-6926b2343?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=ios_app</t>
+  </si>
+  <si>
+    <t>https://github.com/jayjariwala123</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1OzakOoecwLeF4JQvcCMpiDi7eleARYH3</t>
+  </si>
+  <si>
+    <t>App Dev and Sponsorship</t>
+  </si>
+  <si>
+    <t>javintrivedi007@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Javin Trivedi </t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/javintrivedi</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/javintrivedi</t>
+  </si>
+  <si>
+    <t>https://github.com/javintrivedi</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=17G9INhn8nv8wBhZFWhxbglqAvKiWFgLc</t>
+  </si>
+  <si>
+    <t>Events</t>
+  </si>
+  <si>
+    <t>agrimsharman@gmail.com</t>
+  </si>
+  <si>
+    <t>Agrim Sharma</t>
+  </si>
+  <si>
+    <t>agrim_sharma_og</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/agrim-sharma-999566335?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
+  </si>
+  <si>
+    <t>https://github.com/agrim-git-hub</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1QWDIlNDkpX394cfWQGf5g6NV6KF_juSm</t>
+  </si>
+  <si>
+    <t>tusharika.suman6@gmail.com</t>
+  </si>
+  <si>
+    <t>Tusharika Suman</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/tusharika.jpeg/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/tusharika-suman-328497270/</t>
+  </si>
+  <si>
+    <t>https://github.com/tusharikasuman</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=1y4-b5OoIHCt2Fldzw65TenN2BXTa8CQc</t>
+  </si>
+  <si>
+    <t>ac7959@srmist.edu.in</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ABHISTA CHAKRABORTY </t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/asey_abhi.nx/</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/abhista-chakraborty-b47029321/</t>
+  </si>
+  <si>
+    <t>https://github.com/Abhista-111005</t>
+  </si>
+  <si>
+    <t>https://drive.google.com/open?id=16zB1HxD03ljNwqCkFzg0wl7k1gkC7We1</t>
+  </si>
+  <si>
+    <t>roopa192004@gmail.com</t>
+  </si>
+  <si>
+    <t>Roopa K</t>
+  </si>
+  <si>
     <t>Associate</t>
-  </si>
-  <si>
-    <t>https://www.instagram.com/justanother.simrann?igsh=MWVncndtM2swNnJ4dw%3D%3D&amp;utm_source=qr</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/simran-nayak-865692297?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=ios_app</t>
-  </si>
-  <si>
-    <t>https://github.com/simrann130904?tab=repositories</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/open?id=1SXRdcVF9FQYYoQldNtodKB_xiCPzaOHE</t>
-  </si>
-  <si>
-    <t>PR</t>
-  </si>
-  <si>
-    <t>christin.kjoseph@gmail.com</t>
-  </si>
-  <si>
-    <t>Christin Kurian Joseph</t>
-  </si>
-  <si>
-    <t>Technical</t>
-  </si>
-  <si>
-    <t>Member</t>
-  </si>
-  <si>
-    <t>https://www.instagram.com/christin._.kj?igsh=MWwwcG02ZTl6YXlyNg==</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/christin-joseph-a12a39252?</t>
-  </si>
-  <si>
-    <t>https://github.com/ChristinJoseph</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/open?id=1mgAX4od3RahXehy42KVxSZ3eA5pFRv6s</t>
-  </si>
-  <si>
-    <t>Web Dev</t>
-  </si>
-  <si>
-    <t>priyanshuvasudev2005@gmail.com</t>
-  </si>
-  <si>
-    <t>Priyanshu Vasudev</t>
-  </si>
-  <si>
-    <t>Board Member</t>
-  </si>
-  <si>
-    <t>https://www.instagram.com/priyanshu.vasudev/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/priyanshu-vasudev-off/</t>
-  </si>
-  <si>
-    <t>https://github.com/Priyanshu2608</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/open?id=1ZxcPvrcPgjfsAxP7CrYr6JdEiQIhWm_8</t>
-  </si>
-  <si>
-    <t>Technical Lead</t>
-  </si>
-  <si>
-    <t>jjariwala111@gmail.com</t>
-  </si>
-  <si>
-    <t>Jay Jariwala</t>
-  </si>
-  <si>
-    <t>Both</t>
-  </si>
-  <si>
-    <t>https://www.instagram.com/thisisjjaay?igsh=NXlnYWdnZW5xMmxr&amp;utm_source=qr</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/jay-jariwala-6926b2343?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=ios_app</t>
-  </si>
-  <si>
-    <t>https://github.com/jayjariwala123</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/open?id=1OzakOoecwLeF4JQvcCMpiDi7eleARYH3</t>
-  </si>
-  <si>
-    <t>App Dev and Sponsorship</t>
-  </si>
-  <si>
-    <t>javintrivedi007@gmail.com</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Javin Trivedi </t>
-  </si>
-  <si>
-    <t>https://www.instagram.com/javintrivedi</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/javintrivedi</t>
-  </si>
-  <si>
-    <t>https://github.com/javintrivedi</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/open?id=17G9INhn8nv8wBhZFWhxbglqAvKiWFgLc</t>
-  </si>
-  <si>
-    <t>Events</t>
-  </si>
-  <si>
-    <t>agrimsharman@gmail.com</t>
-  </si>
-  <si>
-    <t>Agrim Sharma</t>
-  </si>
-  <si>
-    <t>agrim_sharma_og</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/agrim-sharma-999566335?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=android_app</t>
-  </si>
-  <si>
-    <t>https://github.com/agrim-git-hub</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/open?id=1QWDIlNDkpX394cfWQGf5g6NV6KF_juSm</t>
-  </si>
-  <si>
-    <t>tusharika.suman6@gmail.com</t>
-  </si>
-  <si>
-    <t>Tusharika Suman</t>
-  </si>
-  <si>
-    <t>https://www.instagram.com/tusharika.jpeg/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/tusharika-suman-328497270/</t>
-  </si>
-  <si>
-    <t>https://github.com/tusharikasuman</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/open?id=1y4-b5OoIHCt2Fldzw65TenN2BXTa8CQc</t>
-  </si>
-  <si>
-    <t>ac7959@srmist.edu.in</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ABHISTA CHAKRABORTY </t>
-  </si>
-  <si>
-    <t>https://www.instagram.com/asey_abhi.nx/</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/abhista-chakraborty-b47029321/</t>
-  </si>
-  <si>
-    <t>https://github.com/Abhista-111005</t>
-  </si>
-  <si>
-    <t>https://drive.google.com/open?id=16zB1HxD03ljNwqCkFzg0wl7k1gkC7We1</t>
-  </si>
-  <si>
-    <t>roopa192004@gmail.com</t>
-  </si>
-  <si>
-    <t>Roopa K</t>
   </si>
   <si>
     <t>https://www.instagram.com/roopa.539?igsh=MWN6NnhsN24xZms2Yg==</t>
@@ -1342,22 +1342,22 @@
         <v>12</v>
       </c>
       <c r="E3" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="G3" s="10" t="s">
+      <c r="H3" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="11" t="s">
         <v>25</v>
-      </c>
-      <c r="J3" s="11" t="s">
-        <v>26</v>
       </c>
     </row>
     <row r="4">
@@ -1365,31 +1365,31 @@
         <v>45848.55593174769</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="D4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="13" t="s">
+      <c r="E4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="F4" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="14" t="s">
+      <c r="G4" s="14" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="14" t="s">
+      <c r="H4" s="14" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="I4" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="J4" s="15" t="s">
         <v>34</v>
-      </c>
-      <c r="J4" s="15" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="5">
@@ -1397,31 +1397,31 @@
         <v>45848.55733952546</v>
       </c>
       <c r="B5" s="17" t="s">
+        <v>35</v>
+      </c>
+      <c r="C5" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="C5" s="17" t="s">
+      <c r="D5" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="D5" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E5" s="17" t="s">
+      <c r="F5" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="F5" s="18" t="s">
+      <c r="G5" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="H5" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="I5" s="18" t="s">
         <v>41</v>
       </c>
-      <c r="I5" s="18" t="s">
+      <c r="J5" s="19" t="s">
         <v>42</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="6">
@@ -1429,31 +1429,31 @@
         <v>45848.56112861111</v>
       </c>
       <c r="B6" s="13" t="s">
+        <v>43</v>
+      </c>
+      <c r="C6" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="D6" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="D6" s="13" t="s">
+      <c r="E6" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F6" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F6" s="14" t="s">
+      <c r="G6" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="H6" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="I6" s="14" t="s">
         <v>49</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="J6" s="15" t="s">
         <v>50</v>
-      </c>
-      <c r="J6" s="15" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="7">
@@ -1461,10 +1461,10 @@
         <v>45848.56681491898</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="C7" s="17" t="s">
         <v>52</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>53</v>
       </c>
       <c r="D7" s="17" t="s">
         <v>12</v>
@@ -1473,19 +1473,19 @@
         <v>13</v>
       </c>
       <c r="F7" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="G7" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="H7" s="18" t="s">
         <v>55</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="I7" s="18" t="s">
         <v>56</v>
       </c>
-      <c r="I7" s="18" t="s">
+      <c r="J7" s="19" t="s">
         <v>57</v>
-      </c>
-      <c r="J7" s="19" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="8">
@@ -1493,31 +1493,31 @@
         <v>45848.56939878472</v>
       </c>
       <c r="B8" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="D8" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F8" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D8" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E8" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F8" s="13" t="s">
+      <c r="G8" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="H8" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="I8" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="I8" s="14" t="s">
-        <v>64</v>
-      </c>
       <c r="J8" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="9">
@@ -1525,31 +1525,31 @@
         <v>45848.572819953704</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>64</v>
+      </c>
+      <c r="C9" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="D9" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E9" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="F9" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E9" s="17" t="s">
-        <v>30</v>
-      </c>
-      <c r="F9" s="18" t="s">
+      <c r="G9" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="H9" s="18" t="s">
         <v>68</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="I9" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="I9" s="18" t="s">
-        <v>70</v>
-      </c>
       <c r="J9" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10">
@@ -1557,31 +1557,31 @@
         <v>45848.5840966088</v>
       </c>
       <c r="B10" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C10" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="D10" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="13" t="s">
-        <v>29</v>
-      </c>
-      <c r="E10" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F10" s="14" t="s">
+      <c r="G10" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="H10" s="14" t="s">
         <v>74</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="I10" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="I10" s="14" t="s">
-        <v>76</v>
-      </c>
       <c r="J10" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="11">
@@ -1589,16 +1589,16 @@
         <v>45848.58558403935</v>
       </c>
       <c r="B11" s="17" t="s">
+        <v>76</v>
+      </c>
+      <c r="C11" s="17" t="s">
         <v>77</v>
       </c>
-      <c r="C11" s="17" t="s">
+      <c r="D11" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E11" s="17" t="s">
         <v>78</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="E11" s="17" t="s">
-        <v>21</v>
       </c>
       <c r="F11" s="18" t="s">
         <v>79</v>
@@ -1630,7 +1630,7 @@
         <v>12</v>
       </c>
       <c r="E12" s="13" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="F12" s="14" t="s">
         <v>86</v>
@@ -1645,7 +1645,7 @@
         <v>89</v>
       </c>
       <c r="J12" s="15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13">
@@ -1659,10 +1659,10 @@
         <v>91</v>
       </c>
       <c r="D13" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E13" s="17" t="s">
         <v>29</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>30</v>
       </c>
       <c r="F13" s="18" t="s">
         <v>92</v>
@@ -1677,7 +1677,7 @@
         <v>95</v>
       </c>
       <c r="J13" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="14">
@@ -1691,10 +1691,10 @@
         <v>97</v>
       </c>
       <c r="D14" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" s="13" t="s">
         <v>29</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>30</v>
       </c>
       <c r="F14" s="14" t="s">
         <v>98</v>
@@ -1723,10 +1723,10 @@
         <v>103</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E15" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" s="18" t="s">
         <v>104</v>
@@ -1755,7 +1755,7 @@
         <v>110</v>
       </c>
       <c r="D16" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E16" s="13" t="s">
         <v>13</v>
@@ -1787,10 +1787,10 @@
         <v>116</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E17" s="17" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="F17" s="18" t="s">
         <v>117</v>
@@ -1822,7 +1822,7 @@
         <v>12</v>
       </c>
       <c r="E18" s="13" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F18" s="14" t="s">
         <v>124</v>
@@ -1851,10 +1851,10 @@
         <v>130</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E19" s="17" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="F19" s="18" t="s">
         <v>131</v>
@@ -1869,7 +1869,7 @@
         <v>134</v>
       </c>
       <c r="J19" s="19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="20">
@@ -1883,7 +1883,7 @@
         <v>136</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E20" s="13" t="s">
         <v>13</v>
@@ -1901,7 +1901,7 @@
         <v>140</v>
       </c>
       <c r="J20" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21">
@@ -1918,7 +1918,7 @@
         <v>12</v>
       </c>
       <c r="E21" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F21" s="18" t="s">
         <v>143</v>
@@ -1947,10 +1947,10 @@
         <v>148</v>
       </c>
       <c r="D22" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E22" s="13" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="F22" s="14" t="s">
         <v>149</v>
@@ -1982,7 +1982,7 @@
         <v>12</v>
       </c>
       <c r="E23" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F23" s="18" t="s">
         <v>155</v>
@@ -1997,7 +1997,7 @@
         <v>158</v>
       </c>
       <c r="J23" s="19" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24">
@@ -2014,7 +2014,7 @@
         <v>12</v>
       </c>
       <c r="E24" s="13" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="F24" s="14" t="s">
         <v>161</v>
@@ -2043,10 +2043,10 @@
         <v>166</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E25" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F25" s="18" t="s">
         <v>167</v>
@@ -2075,10 +2075,10 @@
         <v>173</v>
       </c>
       <c r="D26" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E26" s="13" t="s">
         <v>29</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>30</v>
       </c>
       <c r="F26" s="14" t="s">
         <v>174</v>
@@ -2110,7 +2110,7 @@
         <v>12</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="F27" s="18" t="s">
         <v>180</v>
@@ -2139,10 +2139,10 @@
         <v>185</v>
       </c>
       <c r="D28" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E28" s="13" t="s">
         <v>29</v>
-      </c>
-      <c r="E28" s="13" t="s">
-        <v>30</v>
       </c>
       <c r="F28" s="14" t="s">
         <v>186</v>
@@ -2174,7 +2174,7 @@
         <v>12</v>
       </c>
       <c r="E29" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F29" s="18" t="s">
         <v>192</v>
@@ -2189,7 +2189,7 @@
         <v>195</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30">
@@ -2203,10 +2203,10 @@
         <v>197</v>
       </c>
       <c r="D30" s="13" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E30" s="13" t="s">
-        <v>21</v>
+        <v>78</v>
       </c>
       <c r="F30" s="14" t="s">
         <v>198</v>
@@ -2221,7 +2221,7 @@
         <v>201</v>
       </c>
       <c r="J30" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="31">
@@ -2238,7 +2238,7 @@
         <v>12</v>
       </c>
       <c r="E31" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F31" s="18" t="s">
         <v>204</v>
@@ -2253,7 +2253,7 @@
         <v>207</v>
       </c>
       <c r="J31" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32">
@@ -2267,10 +2267,10 @@
         <v>209</v>
       </c>
       <c r="D32" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="E32" s="13" t="s">
         <v>29</v>
-      </c>
-      <c r="E32" s="13" t="s">
-        <v>30</v>
       </c>
       <c r="F32" s="14" t="s">
         <v>210</v>
@@ -2285,7 +2285,7 @@
         <v>213</v>
       </c>
       <c r="J32" s="15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33">
@@ -2299,10 +2299,10 @@
         <v>215</v>
       </c>
       <c r="D33" s="17" t="s">
+        <v>28</v>
+      </c>
+      <c r="E33" s="17" t="s">
         <v>29</v>
-      </c>
-      <c r="E33" s="17" t="s">
-        <v>30</v>
       </c>
       <c r="F33" s="18" t="s">
         <v>216</v>
@@ -2331,10 +2331,10 @@
         <v>221</v>
       </c>
       <c r="D34" s="21" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="E34" s="21" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F34" s="22" t="s">
         <v>222</v>

</xml_diff>